<commit_message>
Nova versão atualizada, sistema de requisição 80% completo
</commit_message>
<xml_diff>
--- a/db/registros_requisicoes.xlsx
+++ b/db/registros_requisicoes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,250 +446,816 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Nome do Cliente</t>
+          <t>CNPJ</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Início de Contrato</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Vigência</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Motivo</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Faturamento</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Cliente</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Comercial</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Contrato</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Envio</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Endereço</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>E-mail</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Quantidade</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Modelo</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Customização</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Tipo de Problema</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Tratativa</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Carregador</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Cabo</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Fatura</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Valor</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Forma de Pgamento</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Observações</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Validação</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Forma de Pagamento</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>REQ00011</t>
+          <t>REQ00002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>28-03-2024 09:46</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Nome do Cliente</t>
-        </is>
+          <t>03-04-2024 12:01</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>12345678912315</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Manutenção</t>
+          <t>12/01/1998</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Sem vigência</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Aquisição Nova</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Sompo</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Thiago</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Retornável</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Correio</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Rua Haiti, 129, Santo André</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>inteligencia@grupogoldensat.com.br</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>45</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>GS 419</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Caixa blindada</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>30</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
           <t>Com custo</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Modelo</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Customização</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Tipo de Problema</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Tratativa</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Aprovada</t>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>ENTREGA</t>
+        </is>
+      </c>
+      <c r="X2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>Em Aberto</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>Boleto</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2803240957</t>
+          <t>REQ00004</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>28-03-2024 09:57</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Grupo GoldenSat</t>
-        </is>
+          <t>03-04-2024 12:05</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>12345678912315</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Manutenção</t>
+          <t>12/01/1998</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>Sem vigência</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Aquisição Nova</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Eurico</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Thiago</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Descartável</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Retirada na base</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Rua dos Vianas,3545</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Eurico</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>comercial@grupogoldensat.com.br</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>2</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>GS 410</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Caixa de papelão</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
+        <v>30</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
           <t>Com custo</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>branco</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>555</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>222</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Rejeitada</t>
+      <c r="U3" t="n">
+        <v>1998</v>
+      </c>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>ENTREGA</t>
+        </is>
+      </c>
+      <c r="X3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Em Aberto</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>123</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>REQ00016</t>
+          <t>REQ00006</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>28-03-2024 10:00</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Bla bla bla</t>
-        </is>
+          <t>03-04-2024 12:06</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>12312313213213</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Manutenção</t>
+          <t>12/01/1998</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>Sem vigência</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Aquisição Nova</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Eurico</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Retornável</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Correio</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Rua dos Vianas,3545</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Eurico</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>comercial@grupogoldensat.com.br</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>2</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>GS 410</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Caixa de papelão</t>
+        </is>
+      </c>
+      <c r="Q4" t="n">
+        <v>30</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
           <t>Com custo</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Automotivo</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Ferrariazika</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Não tem</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Algo aconteceu</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Aprovada</t>
+      <c r="U4" t="n">
+        <v>123</v>
+      </c>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>ENTREGA</t>
+        </is>
+      </c>
+      <c r="X4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>Em Aberto</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>Boleto</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>REQ00018</t>
+          <t>REQ00008</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>28-03-2024 10:55</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Grupo GoldenSat</t>
-        </is>
+          <t>03-04-2024 12:11</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Devolução/Estoque</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Sem custo</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>fas</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>dsad</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>gsa</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>gsa</t>
+          <t>Retornável</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Rejeitada</t>
+          <t>Correio</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>GS 410</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Caixa de papelão</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U5" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="X5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>Em Aberto</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>REQ00010</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>03-04-2024 12:20</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>12345678912315</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>12/01/1998</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Sem vigência</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Aquisição Nova</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Testezinho</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Retornável</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Correio</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Rua Haiti, 129, Santo André</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>BASE.SOMPO@GRUPOGOLDENSAT.COM.BR</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>1231</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>GS 410</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Caixa de papelão</t>
+        </is>
+      </c>
+      <c r="Q6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Com custo</t>
+        </is>
+      </c>
+      <c r="U6" t="n">
+        <v>1080</v>
+      </c>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>ENTREGA</t>
+        </is>
+      </c>
+      <c r="X6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>Em Aberto</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>Boleto</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>REQ00012</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>03-04-2024 12:21</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>312321</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>3213</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>213213</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>12321321</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Retornável</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Correio</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>32132</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>13123</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>21321</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>13213</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>GS 410</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Caixa de papelão</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>123213</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>12312</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>31232</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>1321</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>32131</t>
+        </is>
+      </c>
+      <c r="X7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>Em Aberto</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>311</t>
         </is>
       </c>
     </row>

</xml_diff>